<commit_message>
update the status of review record for traceability matrix
</commit_message>
<xml_diff>
--- a/Documents/External/ReviewRecords/Review_Sheet_Traceability_Matrix_CommLib.xlsx
+++ b/Documents/External/ReviewRecords/Review_Sheet_Traceability_Matrix_CommLib.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="28502"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="28209"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/310235388/Desktop/Traceability/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/310088528p/dev/android-commlib-workspace/Source/commlib/Documents/External/ReviewRecords/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="33600" windowHeight="19780" tabRatio="904" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19020" tabRatio="904"/>
   </bookViews>
   <sheets>
     <sheet name="Title Page" sheetId="3" r:id="rId1"/>
@@ -1099,7 +1099,7 @@
   <sheetPr codeName="Sheet4" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView view="pageLayout" zoomScale="80" zoomScalePageLayoutView="80" workbookViewId="0">
+    <sheetView tabSelected="1" view="pageLayout" zoomScale="80" workbookViewId="0">
       <selection activeCell="A6" sqref="A6:H6"/>
     </sheetView>
   </sheetViews>
@@ -1283,7 +1283,7 @@
   </sheetPr>
   <dimension ref="A1:H56"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="B1" workbookViewId="0">
+    <sheetView view="pageLayout" topLeftCell="A4" workbookViewId="0">
       <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>

</xml_diff>